<commit_message>
edit order of nurses on the list
</commit_message>
<xml_diff>
--- a/forms/release/onco_hcw_questionnaire.xlsx
+++ b/forms/release/onco_hcw_questionnaire.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/trop0451_ox_ac_uk/Documents/sc_onco_facility_study/questionnaire/xlsform/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2781" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5AE2543-B1C3-4A8E-8BBB-8CE67122BEFC}"/>
+  <xr:revisionPtr revIDLastSave="2783" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9784AA51-9377-4872-B085-1476185228D3}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -402,49 +402,49 @@
     <t>hcw01</t>
   </si>
   <si>
+    <t>Audrey Zoe</t>
+  </si>
+  <si>
+    <t>hcw02</t>
+  </si>
+  <si>
+    <t>Cecile Charlette</t>
+  </si>
+  <si>
+    <t>hcw03</t>
+  </si>
+  <si>
+    <t>Ginette Leon</t>
+  </si>
+  <si>
+    <t>hcw04</t>
+  </si>
+  <si>
+    <t>Irene Dorothee</t>
+  </si>
+  <si>
+    <t>hcw05</t>
+  </si>
+  <si>
     <t>Lucie Quilindo</t>
   </si>
   <si>
-    <t>hcw02</t>
+    <t>hcw06</t>
+  </si>
+  <si>
+    <t>Maggie Morel</t>
+  </si>
+  <si>
+    <t>hcw07</t>
+  </si>
+  <si>
+    <t>Phylis Nunoo</t>
+  </si>
+  <si>
+    <t>hcw08</t>
   </si>
   <si>
     <t>Yvonne Telemaque</t>
-  </si>
-  <si>
-    <t>hcw03</t>
-  </si>
-  <si>
-    <t>Maggie Morel</t>
-  </si>
-  <si>
-    <t>hcw04</t>
-  </si>
-  <si>
-    <t>Cecile Charlette</t>
-  </si>
-  <si>
-    <t>hcw05</t>
-  </si>
-  <si>
-    <t>Audrey Zoe</t>
-  </si>
-  <si>
-    <t>hcw06</t>
-  </si>
-  <si>
-    <t>Ginette Leon</t>
-  </si>
-  <si>
-    <t>hcw07</t>
-  </si>
-  <si>
-    <t>Irene Dorothee</t>
-  </si>
-  <si>
-    <t>hcw08</t>
-  </si>
-  <si>
-    <t>Phylis Nunoo</t>
   </si>
   <si>
     <t>hcw09</t>
@@ -2180,7 +2180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
       <selection pane="bottomLeft"/>
@@ -3086,7 +3086,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D366" sqref="D366"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.6"/>
@@ -9033,7 +9033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310AA5A0-4D6B-4099-B591-C5C0F41F7863}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -9088,7 +9088,7 @@
         <v>486</v>
       </c>
       <c r="H2" s="4">
-        <v>2025050802</v>
+        <v>2025050803</v>
       </c>
     </row>
   </sheetData>

</xml_diff>